<commit_message>
Ajout temps réalisation fichier Correction
</commit_message>
<xml_diff>
--- a/tp03/Correction TP3(R).xlsx
+++ b/tp03/Correction TP3(R).xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855CB62F-D5D3-AE46-B400-E52C40A362D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{855CB62F-D5D3-AE46-B400-E52C40A362D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BDF0550-7E21-4DD7-A794-21C21AB22B69}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="20940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23115" yWindow="75" windowWidth="24300" windowHeight="16770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Numéro de dossier (NI):</t>
   </si>
   <si>
-    <t xml:space="preserve">Temps de réalisation : </t>
-  </si>
-  <si>
     <t>Note :</t>
   </si>
   <si>
@@ -267,6 +264,9 @@
   </si>
   <si>
     <t>Charles-Edouard Sarault</t>
+  </si>
+  <si>
+    <t>Temps de réalisation :  Environ 10-15 heure incluant optimisation</t>
   </si>
 </sst>
 </file>
@@ -708,49 +708,49 @@
   <dimension ref="A1:J115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.1640625" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
-    <col min="4" max="4" width="90.83203125" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" customWidth="1"/>
-    <col min="8" max="8" width="3.6640625" customWidth="1"/>
+    <col min="1" max="1" width="58.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="90.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
     <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="6.1640625" customWidth="1"/>
-    <col min="12" max="12" width="11.5" customWidth="1"/>
+    <col min="10" max="10" width="6.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>111124001</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
         <v>536889657</v>
       </c>
@@ -759,12 +759,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>4</v>
       </c>
       <c r="D7" s="5">
         <f>C25+C36+C46+C60+C71+C82+C91+C109+C115</f>
@@ -774,9 +774,9 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="5">
         <f>B25+B36+B46+B60+B71+B82+B91+B109+B115</f>
@@ -786,106 +786,106 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="6" t="s">
+    </row>
+    <row r="13" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="B15" s="8">
+        <v>1</v>
+      </c>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="B15" s="8">
-        <v>1</v>
-      </c>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>11</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="9" t="s">
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
-        <v>15</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
-        <v>19</v>
-      </c>
       <c r="B24" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" s="1">
         <f>SUM(B15:B24)</f>
@@ -896,75 +896,75 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
     </row>
-    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="B31">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
     </row>
-    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B36" s="1">
         <f>SUM(B28:B35)</f>
@@ -975,71 +975,71 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="1"/>
     </row>
-    <row r="38" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
     </row>
-    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
-        <v>29</v>
-      </c>
       <c r="B42">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
     </row>
-    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B46" s="1">
         <f>SUM(B39:B45)</f>
@@ -1050,108 +1050,108 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
     </row>
-    <row r="49" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="9" t="s">
+      <c r="B50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="9" t="s">
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="B52">
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="9" t="s">
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="9" t="s">
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="9" t="s">
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A57" s="7" t="s">
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="7" t="s">
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="B59">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B60" s="1">
         <f>SUM(B49:B59)</f>
@@ -1162,80 +1162,80 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A62" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
     </row>
-    <row r="63" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="9" t="s">
+      <c r="B64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A65" s="9" t="s">
+      <c r="B65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="9" t="s">
+      <c r="B66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="9" t="s">
+      <c r="B67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="9" t="s">
+      <c r="B69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="9" t="s">
-        <v>49</v>
-      </c>
       <c r="B70">
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B71" s="1">
         <f>SUM(B63:B70)</f>
@@ -1246,75 +1246,75 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
     </row>
-    <row r="74" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="9" t="s">
+      <c r="B75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A76" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A77" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A78" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="9" t="s">
+      <c r="B79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A80" s="9" t="s">
-        <v>54</v>
-      </c>
       <c r="B80">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="9"/>
     </row>
-    <row r="82" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B82" s="1">
         <f>SUM(B74:B81)</f>
@@ -1325,47 +1325,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="14"/>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
     </row>
-    <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B87">
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B88">
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B89">
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="10"/>
       <c r="B90" s="1"/>
     </row>
-    <row r="91" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B91" s="1">
         <f>SUM(B86:B90)</f>
@@ -1376,131 +1376,131 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A93" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
     </row>
-    <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A95" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" s="14" t="s">
+      <c r="B95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="B95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" s="14" t="s">
-        <v>62</v>
       </c>
       <c r="B96">
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="14" t="s">
         <v>63</v>
-      </c>
-      <c r="B97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A98" s="14" t="s">
-        <v>64</v>
       </c>
       <c r="B98">
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="14" t="s">
         <v>65</v>
-      </c>
-      <c r="B99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A100" s="14" t="s">
-        <v>66</v>
       </c>
       <c r="B100">
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A102" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B101">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A102" s="14" t="s">
+      <c r="B102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A103" s="14" t="s">
         <v>68</v>
-      </c>
-      <c r="B102">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" s="14" t="s">
-        <v>69</v>
       </c>
       <c r="B103">
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B104">
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B105">
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B106">
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B107">
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="14"/>
     </row>
-    <row r="109" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B109" s="1">
         <f>SUM(B94:B108)</f>
@@ -1511,39 +1511,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="11"/>
       <c r="B110" s="1"/>
     </row>
-    <row r="111" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A111" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
     </row>
-    <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B112">
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B113">
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="10"/>
     </row>
-    <row r="115" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B115" s="1">
         <f>SUM(B112:B114)</f>

</xml_diff>

<commit_message>
Messages modifiées selon captures écran cahier charges
</commit_message>
<xml_diff>
--- a/tp03/Correction TP3(R).xlsx
+++ b/tp03/Correction TP3(R).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{855CB62F-D5D3-AE46-B400-E52C40A362D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BDF0550-7E21-4DD7-A794-21C21AB22B69}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{855CB62F-D5D3-AE46-B400-E52C40A362D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18009F31-7FB8-43A7-B18D-612921C2BF70}"/>
   <bookViews>
-    <workbookView xWindow="23115" yWindow="75" windowWidth="24300" windowHeight="16770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17235" yWindow="0" windowWidth="12990" windowHeight="16770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="80">
   <si>
     <t>Nom et prénom de chaque  coéquipier:</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>Temps de réalisation :  Environ 10-15 heure incluant optimisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                (environ 50% chacun du total)</t>
   </si>
 </sst>
 </file>
@@ -708,7 +711,7 @@
   <dimension ref="A1:J115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,6 +778,9 @@
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="C8" s="4" t="s">
         <v>4</v>
       </c>

</xml_diff>